<commit_message>
indentfoutje eruit gehaald + excel sheet geupdatet
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Updates                               \                      Oplossingstijd (s)</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>copy ipv deepcopy</t>
+  </si>
+  <si>
+    <t>Bij move: tuple-&gt;list-&gt;bewerken-&gt;tuple (dus maar 1x naar list en terug)</t>
   </si>
 </sst>
 </file>
@@ -70,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,15 +167,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.4387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -266,6 +270,23 @@
       </c>
       <c r="E6" s="3" t="n">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Patrick's deel van presentatie toegevoegd
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Updates                               \                      Oplossingstijd (s)</t>
   </si>
@@ -35,28 +35,25 @@
     <t>1 zet kan uit meerdere stappen bestaan</t>
   </si>
   <si>
-    <t>Bord: lijst met lijsten</t>
+    <t>originele situatie</t>
   </si>
   <si>
     <t>&gt;600</t>
   </si>
   <si>
-    <t>~300</t>
-  </si>
-  <si>
-    <t>Bord tuple met tuples</t>
-  </si>
-  <si>
-    <t>Alleen meerdere stappen zetten als het vorige aantal kon</t>
-  </si>
-  <si>
-    <t>deepcopy alleen bij verplaatsing</t>
+    <t>tuples ipv lijsten</t>
+  </si>
+  <si>
+    <t>efficiënte stappen</t>
+  </si>
+  <si>
+    <t>efficiënt borden maken</t>
   </si>
   <si>
     <t>copy ipv deepcopy</t>
   </si>
   <si>
-    <t>Bij move: tuple-&gt;list-&gt;bewerken-&gt;tuple (dus maar 1x naar list en terug)</t>
+    <t>efficiënt tuples aanpassen</t>
   </si>
 </sst>
 </file>
@@ -68,7 +65,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -89,6 +86,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,7 +166,445 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0084D1"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bord 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>originele situatie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tuples ipv lijsten</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>efficiënte stappen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>efficiënt borden maken</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>copy ipv deepcopy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>efficiënt tuples aanpassen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bord 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0084d1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>originele situatie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tuples ipv lijsten</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>efficiënte stappen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>efficiënt borden maken</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>copy ipv deepcopy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>efficiënt tuples aanpassen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bord 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>originele situatie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tuples ipv lijsten</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>efficiënte stappen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>efficiënt borden maken</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>copy ipv deepcopy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>efficiënt tuples aanpassen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="61732952"/>
+        <c:axId val="38154187"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="61732952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="38154187"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38154187"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tijd (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="61732952"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>855000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>48960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>586440</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>29160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="855000" y="1674360"/>
+        <a:ext cx="9756000" cy="5995080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -169,8 +614,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -209,13 +654,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
+      <c r="E2" s="2" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.026</v>
@@ -226,7 +671,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>253.7</v>
@@ -240,7 +685,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.016</v>
@@ -257,7 +702,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.003</v>
@@ -274,7 +719,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.002</v>
@@ -297,5 +742,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A* toegevoegd met heuristiek (aantal auto's tussen RedCar en uitgang + aantal stappen)
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Updates                               \                      Oplossingstijd (s)</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>onnodige try/except weggehaald</t>
+  </si>
+  <si>
+    <t>voor oplossing checken voordat bord aan queue wordt toegevoegd</t>
+  </si>
+  <si>
+    <t>vermijden occupiedBy()</t>
+  </si>
+  <si>
+    <t>Heapq: heuristic = numMoves</t>
+  </si>
+  <si>
+    <t>Heapq: heuristic = numMoves + cars between RedCar &amp; exit</t>
   </si>
 </sst>
 </file>
@@ -182,10 +194,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -323,7 +335,7 @@
         <v>0.19</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0.091</v>
+        <v>0.09</v>
       </c>
       <c r="F8" s="5" t="n">
         <v>33</v>
@@ -344,6 +356,77 @@
       </c>
       <c r="F9" s="0" t="n">
         <v>31.9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>38.8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>24.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oplossing voor bord 5 toegevoegd
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -197,7 +197,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -372,7 +372,7 @@
         <v>0.07</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>24.78</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
heuristiek aangepast (tm Level 2: de car die in de weg zit van de car tussen redcar en uitgang)
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="15360" windowHeight="8220" tabRatio="206"/>
+    <workbookView windowWidth="19575" windowHeight="8655" tabRatio="103"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>Updates                               \                      Oplossingstijd (s)</t>
   </si>
@@ -48,37 +48,7 @@
     <t>Opgelost in: (Aantal stappen)</t>
   </si>
   <si>
-    <t>originele situatie</t>
-  </si>
-  <si>
     <t>&gt;600</t>
-  </si>
-  <si>
-    <t>tuples ipv lijsten</t>
-  </si>
-  <si>
-    <t>efficiënte stappen</t>
-  </si>
-  <si>
-    <t>efficiënt borden maken</t>
-  </si>
-  <si>
-    <t>copy ipv deepcopy</t>
-  </si>
-  <si>
-    <t>efficiënt tuples aanpassen</t>
-  </si>
-  <si>
-    <t>nog efficientere stappen</t>
-  </si>
-  <si>
-    <t>onnodige try/except weggehaald</t>
-  </si>
-  <si>
-    <t>voor oplossing checken voordat bord aan queue wordt toegevoegd</t>
-  </si>
-  <si>
-    <t>vermijden occupiedBy()</t>
   </si>
   <si>
     <t>Heapq: heuristic = numMoves</t>
@@ -125,14 +95,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -146,7 +116,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,26 +125,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="42"/>
+        <bgColor indexed="41"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="45"/>
+        <bgColor indexed="41"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="45"/>
+        <bgColor indexed="45"/>
       </patternFill>
     </fill>
   </fills>
@@ -207,14 +171,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -226,22 +190,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -253,6 +214,74 @@
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Comma[0]" xfId="5" builtinId="6"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="007E0021"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00B3B3B3"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFD320"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF420E"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00004586"/>
+      <rgbColor rgb="00579D1C"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -557,11 +586,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
             <a:gs pos="0">
               <a:srgbClr val="BBD5F0"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="9CBEE0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -588,14 +617,14 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="56.5714285714286" customWidth="1"/>
-    <col min="2" max="9" width="8.57142857142857" customWidth="1"/>
-    <col min="10" max="1027" width="11.5238095238095"/>
+    <col min="1" max="1" width="56.5714285714286"/>
+    <col min="2" max="9" width="8.56190476190476"/>
+    <col min="10" max="1025" width="11.5333333333333"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -650,25 +679,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
+    <row r="4" spans="2:6">
       <c r="B4" s="2">
         <v>0.04</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3">
         <v>300</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
+    <row r="5" spans="2:5">
       <c r="B5">
         <v>0.026</v>
       </c>
@@ -676,10 +699,7 @@
         <v>45.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
+    <row r="6" spans="3:5">
       <c r="C6">
         <v>253.7</v>
       </c>
@@ -690,10 +710,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
+    <row r="7" spans="2:5">
       <c r="B7">
         <v>0.016</v>
       </c>
@@ -707,10 +724,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
+    <row r="8" spans="2:6">
       <c r="B8">
         <v>0.003</v>
       </c>
@@ -725,10 +739,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
+    <row r="9" spans="2:6">
       <c r="B9">
         <v>0.002</v>
       </c>
@@ -745,10 +756,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
+    <row r="10" spans="3:6">
       <c r="C10" s="5">
         <v>0.92</v>
       </c>
@@ -762,10 +770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
+    <row r="11" spans="3:6">
       <c r="C11" s="4">
         <v>0.9</v>
       </c>
@@ -779,10 +784,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
+    <row r="12" spans="3:6">
       <c r="C12">
         <v>0.83</v>
       </c>
@@ -796,10 +798,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
+    <row r="13" spans="3:6">
       <c r="C13" s="4">
         <v>0.8</v>
       </c>
@@ -818,7 +817,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>0.89</v>
@@ -835,7 +834,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>0.87</v>
@@ -852,23 +851,23 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D17" s="4"/>
       <c r="F17" s="7"/>
-      <c r="H17" s="8" t="s">
-        <v>24</v>
+      <c r="H17" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H18" s="9">
         <v>42</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="4:6">
@@ -877,14 +876,14 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>0.86</v>
@@ -901,7 +900,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>0.86</v>
@@ -912,19 +911,19 @@
       <c r="E22" s="1">
         <v>0.05</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>14.2</v>
       </c>
       <c r="H22">
         <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
         <v>0.91</v>
@@ -935,58 +934,58 @@
       <c r="E23" s="1">
         <v>0.04</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>12.2</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
         <v>0.93</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>0.11</v>
       </c>
       <c r="E24" s="1">
         <v>0.04</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <v>10.3</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1">
         <v>0.93</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>0.09</v>
       </c>
       <c r="E25" s="1">
         <v>0.05</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>10.1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
         <v>0.93</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>0.1</v>
       </c>
       <c r="E26" s="1">
         <v>0.04</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="9">
         <v>9.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
In aStarSimulation veranderd dat niet meer een vakje overslaat bij checken of er auto's in de weg staan. + tijden gemeten
</commit_message>
<xml_diff>
--- a/doc/tijden.xlsx
+++ b/doc/tijden.xlsx
@@ -5,10 +5,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19575" windowHeight="8655" tabRatio="103"/>
+    <workbookView windowWidth="11010" windowHeight="8220" tabRatio="284" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74">
   <si>
     <t>Updates                               \                      Oplossingstijd (s)</t>
   </si>
@@ -81,13 +82,25 @@
     <t>Heapq: heuristic = numMoves</t>
   </si>
   <si>
-    <t>Heapq: heuristic = numMoves + 1*(cars between RedCar &amp; exit)</t>
-  </si>
-  <si>
-    <t>Heapq: heuristic = numMoves + 1*(cars between RedCar &amp; exit) + cars in the way of these cars</t>
-  </si>
-  <si>
-    <t>~5GB</t>
+    <t>Heapq: heuristic = numMoves +Level 1</t>
+  </si>
+  <si>
+    <t>Heapq: heuristic = numMoves + Level 2</t>
+  </si>
+  <si>
+    <t>Memory for the one above ^</t>
+  </si>
+  <si>
+    <t>8 MB</t>
+  </si>
+  <si>
+    <t>120 MB</t>
+  </si>
+  <si>
+    <t>5,5 GB</t>
+  </si>
+  <si>
+    <t>6,3 GB</t>
   </si>
   <si>
     <t>Vanaf hier kan niet gegarandeerd worden dat de kortste oplossing wordt gevonden!!</t>
@@ -121,6 +134,111 @@
   </si>
   <si>
     <t>Heapq: heuristic = numMoves + 20*(cars between RedCar &amp; exit)</t>
+  </si>
+  <si>
+    <t>Puzzle no.</t>
+  </si>
+  <si>
+    <t>Grid size</t>
+  </si>
+  <si>
+    <t>State space</t>
+  </si>
+  <si>
+    <t>Solving time (s)</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>Breadth-First</t>
+  </si>
+  <si>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>Puzzle 1</t>
+  </si>
+  <si>
+    <t>6x6</t>
+  </si>
+  <si>
+    <t>$1 \cdot 10^6$</t>
+  </si>
+  <si>
+    <t>$0,80 \pm 0,02$</t>
+  </si>
+  <si>
+    <t>$1,27 \pm 0,02$</t>
+  </si>
+  <si>
+    <t>Puzzle 2</t>
+  </si>
+  <si>
+    <t>$2 \cdot 10^8$</t>
+  </si>
+  <si>
+    <t>$0,13 \pm 0,01$</t>
+  </si>
+  <si>
+    <t>$0,11 \pm 0,01$</t>
+  </si>
+  <si>
+    <t>Puzzle 3</t>
+  </si>
+  <si>
+    <t>$9 \cdot 10^6$</t>
+  </si>
+  <si>
+    <t>$0,07 \pm 0,005$</t>
+  </si>
+  <si>
+    <t>$0,06 \pm 0,005$</t>
+  </si>
+  <si>
+    <t>Puzzle 4</t>
+  </si>
+  <si>
+    <t>9x9</t>
+  </si>
+  <si>
+    <t>$7 \cdot 10^{14}$</t>
+  </si>
+  <si>
+    <t>$25,2 \pm 0,5$</t>
+  </si>
+  <si>
+    <t>$20,3 \pm 0,5$</t>
+  </si>
+  <si>
+    <t>Puzzle 5</t>
+  </si>
+  <si>
+    <t>$1 \cdot 10^{18}$</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>$670 \pm 2$</t>
+  </si>
+  <si>
+    <t>Puzzle 6</t>
+  </si>
+  <si>
+    <t>$6 \cdot 10^{18}$</t>
+  </si>
+  <si>
+    <t>$664 \pm 2$</t>
+  </si>
+  <si>
+    <t>Puzzle 7</t>
+  </si>
+  <si>
+    <t>12x12</t>
+  </si>
+  <si>
+    <t>$9 \cdot 10^{32}$</t>
   </si>
 </sst>
 </file>
@@ -128,14 +246,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
-    <numFmt numFmtId="179" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -208,26 +326,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
@@ -647,10 +765,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
@@ -693,22 +811,22 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>33</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>15</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>21</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>27</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="4">
         <v>22</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>18</v>
       </c>
     </row>
@@ -716,16 +834,16 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>0.04</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>300</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -782,10 +900,10 @@
       <c r="D8">
         <v>1.11</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>0.2</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -797,7 +915,7 @@
       <c r="C9">
         <v>3.35</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9">
@@ -811,16 +929,16 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="7">
         <v>0.92</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="7">
         <v>0.19</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="7">
         <v>0.09</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>33</v>
       </c>
     </row>
@@ -828,7 +946,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>0.9</v>
       </c>
       <c r="D11">
@@ -854,12 +972,12 @@
       <c r="E12">
         <v>0.07</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="2">
         <v>25.4</v>
       </c>
     </row>
     <row r="13" spans="3:6">
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>0.8</v>
       </c>
       <c r="D13">
@@ -868,12 +986,12 @@
       <c r="E13">
         <v>0.07</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>25.2</v>
       </c>
     </row>
     <row r="14" spans="6:6">
-      <c r="F14" s="6"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -899,176 +1017,194 @@
       <c r="C16">
         <v>0.87</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="1">
         <v>0.1</v>
       </c>
       <c r="E16">
         <v>0.05</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="C17">
-        <v>1.1</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.13</v>
+        <v>1.27</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.11</v>
       </c>
       <c r="E17">
-        <v>0.07</v>
-      </c>
-      <c r="F17" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="F17" s="3">
         <v>20.3</v>
       </c>
+      <c r="G17">
+        <v>670</v>
+      </c>
       <c r="H17">
-        <v>392</v>
-      </c>
-      <c r="I17" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="4:6">
-      <c r="D18" s="4"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="8" t="s">
+      <c r="D18" s="1"/>
+      <c r="F18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="F20" s="7"/>
-      <c r="H20" s="1" t="s">
+      <c r="G18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="9" t="s">
+      <c r="H18" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="9">
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="1"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="3"/>
+      <c r="H21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="9">
         <v>42</v>
       </c>
-      <c r="I21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4">
         <v>0.86</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D23" s="4">
         <v>0.09</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="4">
         <v>0.05</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="4">
         <v>17.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1">
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="4">
         <v>0.86</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="4">
         <v>0.08</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E24" s="4">
         <v>0.05</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="9">
         <v>14.2</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>41</v>
       </c>
-      <c r="I23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.91</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.07</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="F24" s="9">
-        <v>12.2</v>
+      <c r="I24" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0.11</v>
-      </c>
-      <c r="E25" s="1">
+        <v>35</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.07</v>
+      </c>
+      <c r="E25" s="4">
         <v>0.04</v>
       </c>
       <c r="F25" s="9">
-        <v>10.3</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="1">
+        <v>36</v>
+      </c>
+      <c r="C26" s="4">
         <v>0.93</v>
       </c>
       <c r="D26" s="9">
-        <v>0.09</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.05</v>
+        <v>0.11</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.04</v>
       </c>
       <c r="F26" s="9">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1">
+        <v>37</v>
+      </c>
+      <c r="C27" s="4">
         <v>0.93</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="9">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="D28" s="10">
         <v>0.1</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E28" s="4">
         <v>0.04</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F28" s="9">
         <v>9.1</v>
       </c>
     </row>
@@ -1080,4 +1216,180 @@
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="B3:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="11.25" outlineLevelCol="6"/>
+  <cols>
+    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
+    <col min="5" max="5" width="15.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="15.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6">
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>